<commit_message>
KIBON-2685 attribute zu excel export hinzufügen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichBGZeitabschnitte.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichBGZeitabschnitte.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B959489-A2A1-4FA6-9FA2-867831BA646D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95867322-093D-4A52-A7FF-22A5EC8A7196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>{nameGemeinde}</t>
   </si>
@@ -45,13 +45,101 @@
   </si>
   <si>
     <t>{repeatRow}</t>
+  </si>
+  <si>
+    <t>{lastenausgleichDatenTitle}</t>
+  </si>
+  <si>
+    <t>{parameterTitle}</t>
+  </si>
+  <si>
+    <t>{referenznummerTitle}</t>
+  </si>
+  <si>
+    <t>{referenznummer}</t>
+  </si>
+  <si>
+    <t>{bfsNummerTitle}</t>
+  </si>
+  <si>
+    <t>{bfsNummer}</t>
+  </si>
+  <si>
+    <t>{nachnameTitle}</t>
+  </si>
+  <si>
+    <t>{nachname}</t>
+  </si>
+  <si>
+    <t>{vornameTitle}</t>
+  </si>
+  <si>
+    <t>{vorname}</t>
+  </si>
+  <si>
+    <t>{geburtsdatumTitle}</t>
+  </si>
+  <si>
+    <t>{geburtsdatum}</t>
+  </si>
+  <si>
+    <t>{vonTitle}</t>
+  </si>
+  <si>
+    <t>{von}</t>
+  </si>
+  <si>
+    <t>{bisTitle}</t>
+  </si>
+  <si>
+    <t>{bis}</t>
+  </si>
+  <si>
+    <t>{institutionTitle}</t>
+  </si>
+  <si>
+    <t>{institution}</t>
+  </si>
+  <si>
+    <t>{betreuungsangebotTypTitle}</t>
+  </si>
+  <si>
+    <t>{betreuungsangebotTyp}</t>
+  </si>
+  <si>
+    <t>{bgPensumTitle}</t>
+  </si>
+  <si>
+    <t>{bgPensum}</t>
+  </si>
+  <si>
+    <t>{keinSelbstbehaltDurchGemeindeTitle}</t>
+  </si>
+  <si>
+    <t>{keinSelbstbehaltDurchGemeinde}</t>
+  </si>
+  <si>
+    <t>{gutscheinTitle}</t>
+  </si>
+  <si>
+    <t>{gutschein}</t>
+  </si>
+  <si>
+    <t>{jahrTitle}</t>
+  </si>
+  <si>
+    <t>{jahr}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="_ &quot;CHF&quot;\ * #,##0.00_ ;_ &quot;CHF&quot;\ * \-#,##0.00_ ;_ &quot;CHF&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="168" formatCode="&quot;CHF&quot;\ #,##0.00"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,8 +147,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -70,6 +195,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -98,10 +229,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -110,9 +246,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
+    <cellStyle name="Prozent 2" xfId="4" xr:uid="{D49F03AA-E03A-4E8D-8E43-917A169A7D56}"/>
+    <cellStyle name="Prozent 3" xfId="2" xr:uid="{E0BCA340-BEA6-4A70-B197-40BE5F4D95F5}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard 2" xfId="3" xr:uid="{9907BC74-2BE0-4700-9733-D73FA1902CFF}"/>
+    <cellStyle name="Standard 3" xfId="1" xr:uid="{E6B6D074-FC9F-4224-AC82-F19DAC56A154}"/>
+    <cellStyle name="Währung 2" xfId="5" xr:uid="{A3CF4752-6CFF-4DD8-BEB5-2CCE0DA3F59B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -424,30 +588,219 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" customWidth="1"/>
-    <col min="18" max="19" width="0" hidden="1" customWidth="1"/>
-    <col min="34" max="35" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21" style="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="0" hidden="1" customWidth="1"/>
+    <col min="32" max="33" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+    </row>
+    <row r="7" spans="1:23" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="18" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="N8" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
KIBON-2685 berechnungen zu excel template hinzufügen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichBGZeitabschnitte.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichBGZeitabschnitte.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95867322-093D-4A52-A7FF-22A5EC8A7196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E544E8-F17D-44C3-8CD7-CC07136FE20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>{nameGemeinde}</t>
   </si>
@@ -129,15 +129,22 @@
   </si>
   <si>
     <t>{jahr}</t>
+  </si>
+  <si>
+    <t>{selbstbehaltGemeindeTitle}</t>
+  </si>
+  <si>
+    <t>{eingabeLastenausgleichTitle}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="_ &quot;CHF&quot;\ * #,##0.00_ ;_ &quot;CHF&quot;\ * \-#,##0.00_ ;_ &quot;CHF&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="168" formatCode="&quot;CHF&quot;\ #,##0.00"/>
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_ &quot;CHF&quot;\ * #,##0.00_ ;_ &quot;CHF&quot;\ * \-#,##0.00_ ;_ &quot;CHF&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
+    <numFmt numFmtId="167" formatCode="_ &quot;CHF&quot;\ * #,##0.00_ ;_ &quot;CHF&quot;\ * \-#,##0.00_ ;_ &quot;CHF&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -185,7 +192,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,8 +211,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -228,16 +241,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -263,20 +290,36 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Prozent 2" xfId="4" xr:uid="{D49F03AA-E03A-4E8D-8E43-917A169A7D56}"/>
     <cellStyle name="Prozent 3" xfId="2" xr:uid="{E0BCA340-BEA6-4A70-B197-40BE5F4D95F5}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="3" xr:uid="{9907BC74-2BE0-4700-9733-D73FA1902CFF}"/>
     <cellStyle name="Standard 3" xfId="1" xr:uid="{E6B6D074-FC9F-4224-AC82-F19DAC56A154}"/>
     <cellStyle name="Währung 2" xfId="5" xr:uid="{A3CF4752-6CFF-4DD8-BEB5-2CCE0DA3F59B}"/>
+    <cellStyle name="Währung 2 2" xfId="6" xr:uid="{B240190E-49D2-4D8C-AF78-2D312B546D84}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -588,30 +631,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W8"/>
+  <dimension ref="A1:Y8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" customWidth="1"/>
     <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" style="12" customWidth="1"/>
     <col min="7" max="7" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" customWidth="1"/>
     <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21" style="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" style="24" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="28.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="0" hidden="1" customWidth="1"/>
-    <col min="32" max="33" width="13.33203125" customWidth="1"/>
+    <col min="14" max="15" width="28.88671875" style="20" customWidth="1"/>
+    <col min="16" max="16" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="0" hidden="1" customWidth="1"/>
+    <col min="34" max="35" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:25" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -625,10 +669,10 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="13"/>
-      <c r="L1" s="5"/>
+      <c r="L1" s="21"/>
       <c r="M1" s="17"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
@@ -637,8 +681,10 @@
       <c r="U1" s="5"/>
       <c r="V1" s="5"/>
       <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -650,10 +696,10 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="13"/>
-      <c r="L2" s="5"/>
+      <c r="L2" s="21"/>
       <c r="M2" s="17"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
@@ -662,8 +708,10 @@
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
       <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -677,10 +725,10 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="13"/>
-      <c r="L3" s="5"/>
+      <c r="L3" s="21"/>
       <c r="M3" s="17"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
@@ -689,8 +737,10 @@
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
       <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>29</v>
       </c>
@@ -706,10 +756,10 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="5"/>
+      <c r="L4" s="21"/>
       <c r="M4" s="17"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
@@ -718,8 +768,10 @@
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
     </row>
-    <row r="7" spans="1:23" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -753,14 +805,20 @@
       <c r="K7" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="25" t="s">
         <v>25</v>
       </c>
       <c r="M7" s="18" t="s">
         <v>27</v>
       </c>
+      <c r="N7" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="O7" s="22" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -794,13 +852,21 @@
       <c r="K8" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L8" s="23" t="s">
         <v>26</v>
       </c>
       <c r="M8" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="19" t="e">
+        <f>IF(L8&lt;&gt;"X",M8*0.2,0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O8" s="19" t="e">
+        <f>IF(L8&lt;&gt;"X",M8*0.8,M8)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P8" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
KIBON-2774 zusätzliche spalten hinzufügen und berechnung in excel
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichBGZeitabschnitte.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichBGZeitabschnitte.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E544E8-F17D-44C3-8CD7-CC07136FE20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32BAC10-CB93-4D01-B516-FF6556F01952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>{nameGemeinde}</t>
   </si>
@@ -135,16 +135,36 @@
   </si>
   <si>
     <t>{eingabeLastenausgleichTitle}</t>
+  </si>
+  <si>
+    <t>{anteilMonat}</t>
+  </si>
+  <si>
+    <t>{anteilMonatTitle}</t>
+  </si>
+  <si>
+    <t>{korrekturTitle}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {isKorrektur}</t>
+  </si>
+  <si>
+    <t>{alteBerechnungTitle}</t>
+  </si>
+  <si>
+    <t>{selbstbehaltProHundertProzentPlatzTitel}</t>
+  </si>
+  <si>
+    <t>{selbstbehaltProHunderProzentPlatz}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_ &quot;CHF&quot;\ * #,##0.00_ ;_ &quot;CHF&quot;\ * \-#,##0.00_ ;_ &quot;CHF&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
-    <numFmt numFmtId="167" formatCode="_ &quot;CHF&quot;\ * #,##0.00_ ;_ &quot;CHF&quot;\ * \-#,##0.00_ ;_ &quot;CHF&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -262,9 +282,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -310,6 +330,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -631,31 +654,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y8"/>
+  <dimension ref="A1:AC8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.21875" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="16.88671875" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21" style="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="28.88671875" style="20" customWidth="1"/>
-    <col min="16" max="16" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="0" hidden="1" customWidth="1"/>
-    <col min="34" max="35" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" style="12" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="12" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21" style="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="15" max="19" width="28.85546875" style="20" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="0" hidden="1" customWidth="1"/>
+    <col min="38" max="39" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:29" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -668,23 +692,27 @@
       <c r="H1" s="9"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="17"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="21"/>
       <c r="N1" s="17"/>
       <c r="O1" s="17"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
       <c r="T1" s="5"/>
       <c r="U1" s="5"/>
       <c r="V1" s="5"/>
       <c r="W1" s="5"/>
       <c r="X1" s="5"/>
       <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -695,23 +723,27 @@
       <c r="H2" s="9"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="17"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="21"/>
       <c r="N2" s="17"/>
       <c r="O2" s="17"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
       <c r="W2" s="5"/>
       <c r="X2" s="5"/>
       <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -724,23 +756,27 @@
       <c r="H3" s="9"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="17"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="21"/>
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>29</v>
       </c>
@@ -755,23 +791,27 @@
       <c r="H4" s="9"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="17"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="21"/>
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="5"/>
     </row>
-    <row r="7" spans="1:25" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -797,28 +837,40 @@
         <v>17</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="L7" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="25" t="s">
+      <c r="M7" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="18" t="s">
+      <c r="N7" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="N7" s="22" t="s">
+      <c r="O7" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="P7" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q7" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="R7" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="O7" s="22" t="s">
+      <c r="S7" s="22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -844,29 +896,42 @@
         <v>18</v>
       </c>
       <c r="I8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="L8" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="L8" s="23" t="s">
+      <c r="M8" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="M8" s="19" t="s">
+      <c r="N8" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="N8" s="19" t="e">
-        <f>IF(L8&lt;&gt;"X",M8*0.2,0)</f>
+      <c r="O8" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="P8" s="19" t="e">
+        <f>IF(O8="","",I8/12*L8*O8)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="O8" s="19" t="e">
-        <f>IF(L8&lt;&gt;"X",M8*0.8,M8)</f>
+      <c r="Q8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R8" s="19" t="e">
+        <f>IF(M8="X",0,IF(O8="",N8*0.2,P8))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="P8" t="s">
+      <c r="S8" s="19" t="e">
+        <f>N8-R8</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T8" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
KIBON-2774 hinzugefügte spalten für alte berechnung rückgängig machen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichBGZeitabschnitte.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichBGZeitabschnitte.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32BAC10-CB93-4D01-B516-FF6556F01952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF32AD0-F819-48B1-A6B3-584EAE136B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-10870" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>{nameGemeinde}</t>
   </si>
@@ -137,25 +137,10 @@
     <t>{eingabeLastenausgleichTitle}</t>
   </si>
   <si>
-    <t>{anteilMonat}</t>
-  </si>
-  <si>
-    <t>{anteilMonatTitle}</t>
-  </si>
-  <si>
     <t>{korrekturTitle}</t>
   </si>
   <si>
-    <t xml:space="preserve"> {isKorrektur}</t>
-  </si>
-  <si>
-    <t>{alteBerechnungTitle}</t>
-  </si>
-  <si>
-    <t>{selbstbehaltProHundertProzentPlatzTitel}</t>
-  </si>
-  <si>
-    <t>{selbstbehaltProHunderProzentPlatz}</t>
+    <t>{isKorrektur}</t>
   </si>
 </sst>
 </file>
@@ -654,32 +639,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC8"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" style="12" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="12" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21" style="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="15" max="19" width="28.85546875" style="20" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="0" hidden="1" customWidth="1"/>
-    <col min="38" max="39" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21" style="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="28.88671875" style="20" customWidth="1"/>
+    <col min="17" max="17" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="0" hidden="1" customWidth="1"/>
+    <col min="35" max="36" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -692,15 +676,15 @@
       <c r="H1" s="9"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="21"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="17"/>
       <c r="N1" s="17"/>
       <c r="O1" s="17"/>
       <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
       <c r="T1" s="5"/>
       <c r="U1" s="5"/>
       <c r="V1" s="5"/>
@@ -708,11 +692,8 @@
       <c r="X1" s="5"/>
       <c r="Y1" s="5"/>
       <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -723,15 +704,15 @@
       <c r="H2" s="9"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="21"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="17"/>
       <c r="N2" s="17"/>
       <c r="O2" s="17"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
@@ -739,11 +720,8 @@
       <c r="X2" s="5"/>
       <c r="Y2" s="5"/>
       <c r="Z2" s="5"/>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="5"/>
-      <c r="AC2" s="5"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -756,15 +734,15 @@
       <c r="H3" s="9"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="21"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="17"/>
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
       <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
@@ -772,11 +750,8 @@
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
-      <c r="AA3" s="5"/>
-      <c r="AB3" s="5"/>
-      <c r="AC3" s="5"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>29</v>
       </c>
@@ -791,15 +766,15 @@
       <c r="H4" s="9"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="21"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="17"/>
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
       <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
@@ -807,11 +782,8 @@
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
       <c r="Z4" s="5"/>
-      <c r="AA4" s="5"/>
-      <c r="AB4" s="5"/>
-      <c r="AC4" s="5"/>
     </row>
-    <row r="7" spans="1:29" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -837,40 +809,31 @@
         <v>17</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L7" s="14" t="s">
+      <c r="K7" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="M7" s="25" t="s">
+      <c r="L7" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="N7" s="18" t="s">
+      <c r="M7" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="O7" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="P7" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q7" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="R7" s="22" t="s">
+      <c r="N7" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="S7" s="22" t="s">
+      <c r="P7" s="22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -896,42 +859,32 @@
         <v>18</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="K8" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="M8" s="23" t="s">
+      <c r="L8" s="23" t="s">
         <v>26</v>
       </c>
+      <c r="M8" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="N8" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="O8" s="19" t="s">
-        <v>39</v>
+        <v>34</v>
+      </c>
+      <c r="O8" s="19" t="e">
+        <f>IF(L8&lt;&gt;"X",M8*0.2,0)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="P8" s="19" t="e">
-        <f>IF(O8="","",I8/12*L8*O8)</f>
+        <f>IF(L8&lt;&gt;"X",M8*0.8,M8)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="Q8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R8" s="19" t="e">
-        <f>IF(M8="X",0,IF(O8="",N8*0.2,P8))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S8" s="19" t="e">
-        <f>N8-R8</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T8" t="s">
+      <c r="Q8" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
KIBON-2774 summen zum report hinzufügen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichBGZeitabschnitte.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichBGZeitabschnitte.xlsx
@@ -8,14 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF32AD0-F819-48B1-A6B3-584EAE136B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1FE126-61E4-4610-98CF-109629C00F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-10870" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-10870" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="2" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="bgPensum">Data!$K$8</definedName>
+    <definedName name="eingabeLastenausgleich">Data!$P$8</definedName>
+    <definedName name="selbstbehaltGemeinde">Data!$O$8</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="7" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>{nameGemeinde}</t>
   </si>
@@ -141,6 +150,12 @@
   </si>
   <si>
     <t>{isKorrektur}</t>
+  </si>
+  <si>
+    <t>Zeilenbeschriftungen</t>
+  </si>
+  <si>
+    <t>Gesamtergebnis</t>
   </si>
 </sst>
 </file>
@@ -269,7 +284,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -318,6 +333,13 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -340,6 +362,157 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Endtner Janik" refreshedDate="44923.421857060188" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{D1678751-48FE-43CD-9775-A547B894D3EF}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A7:P8" sheet="Data"/>
+  </cacheSource>
+  <cacheFields count="16">
+    <cacheField name="{referenznummerTitle}" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="{bfsNummerTitle}" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="{nameGemeindeTitle}" numFmtId="0">
+      <sharedItems count="1">
+        <s v="{nameGemeinde}"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="{nachnameTitle}" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="{vornameTitle}" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="{geburtsdatumTitle}" numFmtId="14">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="{vonTitle}" numFmtId="14">
+      <sharedItems count="1">
+        <s v="{von}"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="{bisTitle}" numFmtId="14">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="{institutionTitle}" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="{betreuungsangebotTypTitle}" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="{bgPensumTitle}" numFmtId="10">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="{keinSelbstbehaltDurchGemeindeTitle}" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="{gutscheinTitle}" numFmtId="164">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="{korrekturTitle}" numFmtId="164">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="{selbstbehaltGemeindeTitle}" numFmtId="164">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="{eingabeLastenausgleichTitle}" numFmtId="164">
+      <sharedItems/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
+  <r>
+    <s v="{referenznummer}"/>
+    <s v="{bfsNummer}"/>
+    <x v="0"/>
+    <s v="{nachname}"/>
+    <s v="{vorname}"/>
+    <s v="{geburtsdatum}"/>
+    <x v="0"/>
+    <s v="{bis}"/>
+    <s v="{institution}"/>
+    <s v="{betreuungsangebotTyp}"/>
+    <s v="{bgPensum}"/>
+    <s v="{keinSelbstbehaltDurchGemeinde}"/>
+    <s v="{gutschein}"/>
+    <s v="{isKorrektur}"/>
+    <e v="#VALUE!"/>
+    <e v="#VALUE!"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B21C51EE-19F9-4A8A-8854-33C6B1863267}" name="PivotTable2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:A6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="6"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -638,6 +811,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6570C638-CD53-4FD0-B2F4-7C9BABE94530}">
+  <dimension ref="A3:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="28" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z8"/>
   <sheetViews>

</xml_diff>

<commit_message>
KIBON-2815 textänderungen lastenausgleich & einfügen des jährlichen BG-Pensums in LastenusgleichZeitabschnitte Excel
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichBGZeitabschnitte.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichBGZeitabschnitte.xlsx
@@ -8,23 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1FE126-61E4-4610-98CF-109629C00F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC9CEA1-F18E-4DC9-9B0D-D1BD5A69BE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-10870" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="2" r:id="rId1"/>
-    <sheet name="Data" sheetId="1" r:id="rId2"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="bgPensum">Data!$K$8</definedName>
-    <definedName name="eingabeLastenausgleich">Data!$P$8</definedName>
-    <definedName name="selbstbehaltGemeinde">Data!$O$8</definedName>
+    <definedName name="bgPensum">Data!$P$8</definedName>
+    <definedName name="eingabeLastenausgleich">Data!$V$8</definedName>
+    <definedName name="selbstbehaltGemeinde">Data!$U$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId3"/>
-  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>{nameGemeinde}</t>
   </si>
@@ -152,10 +148,22 @@
     <t>{isKorrektur}</t>
   </si>
   <si>
-    <t>Zeilenbeschriftungen</t>
-  </si>
-  <si>
-    <t>Gesamtergebnis</t>
+    <t>Monatstart</t>
+  </si>
+  <si>
+    <t>Monatsende</t>
+  </si>
+  <si>
+    <t>Anzahl Tage Monat</t>
+  </si>
+  <si>
+    <t>Anteil Monat</t>
+  </si>
+  <si>
+    <t>Anteil Jahr</t>
+  </si>
+  <si>
+    <t>{jaehrlichesBGPensumTitle}</t>
   </si>
 </sst>
 </file>
@@ -284,7 +292,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -333,13 +341,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -362,157 +363,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Endtner Janik" refreshedDate="44923.421857060188" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{D1678751-48FE-43CD-9775-A547B894D3EF}">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A7:P8" sheet="Data"/>
-  </cacheSource>
-  <cacheFields count="16">
-    <cacheField name="{referenznummerTitle}" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="{bfsNummerTitle}" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="{nameGemeindeTitle}" numFmtId="0">
-      <sharedItems count="1">
-        <s v="{nameGemeinde}"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="{nachnameTitle}" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="{vornameTitle}" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="{geburtsdatumTitle}" numFmtId="14">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="{vonTitle}" numFmtId="14">
-      <sharedItems count="1">
-        <s v="{von}"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="{bisTitle}" numFmtId="14">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="{institutionTitle}" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="{betreuungsangebotTypTitle}" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="{bgPensumTitle}" numFmtId="10">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="{keinSelbstbehaltDurchGemeindeTitle}" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="{gutscheinTitle}" numFmtId="164">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="{korrekturTitle}" numFmtId="164">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="{selbstbehaltGemeindeTitle}" numFmtId="164">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="{eingabeLastenausgleichTitle}" numFmtId="164">
-      <sharedItems/>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
-  <r>
-    <s v="{referenznummer}"/>
-    <s v="{bfsNummer}"/>
-    <x v="0"/>
-    <s v="{nachname}"/>
-    <s v="{vorname}"/>
-    <s v="{geburtsdatum}"/>
-    <x v="0"/>
-    <s v="{bis}"/>
-    <s v="{institution}"/>
-    <s v="{betreuungsangebotTyp}"/>
-    <s v="{bgPensum}"/>
-    <s v="{keinSelbstbehaltDurchGemeinde}"/>
-    <s v="{gutschein}"/>
-    <s v="{isKorrektur}"/>
-    <e v="#VALUE!"/>
-    <e v="#VALUE!"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B21C51EE-19F9-4A8A-8854-33C6B1863267}" name="PivotTable2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:A6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="2">
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="2">
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="2"/>
-    <field x="6"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -811,70 +661,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6570C638-CD53-4FD0-B2F4-7C9BABE94530}">
-  <dimension ref="A3:A6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="28" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:AF8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.21875" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="16.88671875" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21" style="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="28.88671875" style="20" customWidth="1"/>
-    <col min="17" max="17" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="0" hidden="1" customWidth="1"/>
-    <col min="35" max="36" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" style="12" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="12" customWidth="1"/>
+    <col min="9" max="13" width="13.7109375" style="12" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21" style="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21" style="16" customWidth="1"/>
+    <col min="18" max="18" width="11.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="28.85546875" style="20" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="0" hidden="1" customWidth="1"/>
+    <col min="41" max="42" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:32" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -885,26 +699,32 @@
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
       <c r="W1" s="5"/>
       <c r="X1" s="5"/>
       <c r="Y1" s="5"/>
       <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -913,26 +733,32 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
       <c r="W2" s="5"/>
       <c r="X2" s="5"/>
       <c r="Y2" s="5"/>
       <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -943,26 +769,32 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="5"/>
+      <c r="AE3" s="5"/>
+      <c r="AF3" s="5"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>29</v>
       </c>
@@ -975,26 +807,32 @@
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
       <c r="W4" s="5"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
       <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="5"/>
+      <c r="AF4" s="5"/>
     </row>
-    <row r="7" spans="1:26" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1019,32 +857,50 @@
       <c r="H7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="P7" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="25" t="s">
+      <c r="Q7" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="R7" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="18" t="s">
+      <c r="S7" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="N7" s="26" t="s">
+      <c r="T7" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="O7" s="22" t="s">
+      <c r="U7" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="P7" s="22" t="s">
+      <c r="V7" s="22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1069,33 +925,57 @@
       <c r="H8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="11" t="e">
+        <f>EOMONTH(G8,-1)+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J8" s="11" t="e">
+        <f>EOMONTH(H8, 0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K8" s="1" t="e">
+        <f>J8-I8+1</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L8" s="1" t="e">
+        <f>(H8-G8+1)/K8</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M8" s="1" t="e">
+        <f>L8/12</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="P8" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="L8" s="23" t="s">
+      <c r="Q8" s="15" t="e">
+        <f>M8*P8</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R8" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="M8" s="19" t="s">
+      <c r="S8" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="N8" s="19" t="s">
+      <c r="T8" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="O8" s="19" t="e">
-        <f>IF(L8&lt;&gt;"X",M8*0.2,0)</f>
+      <c r="U8" s="19" t="e">
+        <f>IF(R8&lt;&gt;"X",S8*0.2,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="P8" s="19" t="e">
-        <f>IF(L8&lt;&gt;"X",M8*0.8,M8)</f>
+      <c r="V8" s="19" t="e">
+        <f>IF(R8&lt;&gt;"X",S8*0.8,S8)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="W8" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>